<commit_message>
ahora sí terminamos de medir
</commit_message>
<xml_diff>
--- a/TP4/Mediciones.xlsx
+++ b/TP4/Mediciones.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9628E022-5B54-4802-A080-DAACD4A546E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A98E50-955E-4297-BA73-BF492CEF3BAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Caso</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>magnetico, se pierde gran parte</t>
+  </si>
+  <si>
+    <t>Sin núcleo (I2 = 0)</t>
   </si>
 </sst>
 </file>
@@ -341,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -369,6 +372,36 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -382,30 +415,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -694,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,11 +725,11 @@
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -755,20 +764,23 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>28</v>
+      <c r="B3" s="14">
+        <v>93.4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="6">
+        <f>B3/($N$4*C3)</f>
+        <v>2.9730143369566049</v>
+      </c>
+      <c r="E3" s="14">
+        <f>23</f>
+        <v>23</v>
+      </c>
+      <c r="F3" s="14">
+        <f>21.8</f>
+        <v>21.8</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>11</v>
@@ -784,23 +796,22 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4">
-        <f>94</f>
-        <v>94</v>
+      <c r="B4" s="14">
+        <v>93.4</v>
       </c>
       <c r="C4" s="4">
         <v>0.42</v>
       </c>
       <c r="D4" s="6">
         <f>B4/($N$4*C4)</f>
-        <v>0.71240784050657913</v>
-      </c>
-      <c r="E4" s="4">
+        <v>0.70786055641823931</v>
+      </c>
+      <c r="E4" s="14">
         <f>23</f>
         <v>23</v>
       </c>
-      <c r="F4" s="4">
-        <f>21.8</f>
+      <c r="F4" s="14">
+        <f t="shared" ref="F4:F7" si="0">21.8</f>
         <v>21.8</v>
       </c>
       <c r="M4" s="7" t="s">
@@ -818,79 +829,96 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>28</v>
+      <c r="B5" s="14">
+        <v>93.4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="6">
+        <f>B5/($N$4*C5)</f>
+        <v>0.74325358423915122</v>
+      </c>
+      <c r="E5" s="14">
+        <f>23</f>
+        <v>23</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" si="0"/>
+        <v>21.8</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="4">
-        <f>93.2</f>
-        <v>93.2</v>
+      <c r="B6" s="14">
+        <v>93.4</v>
       </c>
       <c r="C6" s="4">
         <v>0.8</v>
       </c>
       <c r="D6" s="6">
         <f>B6/($N$4*C6)</f>
-        <v>0.37083101740411611</v>
-      </c>
-      <c r="E6" s="4">
-        <f>E4</f>
+        <v>0.37162679211957561</v>
+      </c>
+      <c r="E6" s="14">
+        <f>23</f>
         <v>23</v>
       </c>
-      <c r="F6" s="4">
-        <f>F4</f>
+      <c r="F6" s="14">
+        <f t="shared" si="0"/>
         <v>21.8</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
+      <c r="A7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="14">
+        <v>93.4</v>
+      </c>
+      <c r="C7" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D7" s="6">
+        <f>B7/($N$4*C7)</f>
+        <v>0.37162679211957561</v>
+      </c>
+      <c r="E7" s="14">
+        <f>23</f>
+        <v>23</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="0"/>
+        <v>21.8</v>
+      </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15" t="s">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="O8" s="24" t="s">
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="O8" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="24"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -923,58 +951,61 @@
       <c r="J9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="25" t="s">
+      <c r="O9" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" s="18" t="s">
+      <c r="B10" s="12">
+        <v>93.4</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>14.6</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="F10" s="3">
+        <v>200</v>
+      </c>
+      <c r="G10" s="6">
+        <f>D3</f>
+        <v>2.9730143369566049</v>
+      </c>
+      <c r="H10" s="6">
+        <f>G10/(SQRT(J10*I10))</f>
+        <v>0.77609519362771617</v>
+      </c>
+      <c r="I10" s="6">
+        <f>SQRT(B10^2 - (C10*E3)^2)/($N$4*C10)</f>
+        <v>0.98829680833112554</v>
+      </c>
+      <c r="J10" s="6">
+        <f>SQRT((C10*D3*$N$4)^2-(E10*(F3+F10))^2)/(E10*$N$4)</f>
+        <v>14.848296339954329</v>
+      </c>
+      <c r="O10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="19"/>
-      <c r="Q10" s="19"/>
-      <c r="R10" s="20"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="17"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="4">
-        <f>94</f>
-        <v>94</v>
+      <c r="B11" s="12">
+        <v>93.4</v>
       </c>
       <c r="C11" s="4">
         <f>0.45</f>
@@ -992,67 +1023,70 @@
         <v>200</v>
       </c>
       <c r="G11" s="6">
-        <f t="shared" ref="G11" si="0">D4</f>
-        <v>0.71240784050657913</v>
+        <f>D4</f>
+        <v>0.70786055641823931</v>
       </c>
       <c r="H11" s="6">
         <f>G11/(SQRT(J11*I11))</f>
-        <v>0.49556140259133119</v>
+        <v>0.49566243286548706</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" ref="I11" si="1">SQRT(B11^2 - (C11*E4)^2)/($N$4*C11)</f>
-        <v>0.66087117968090037</v>
+        <f>SQRT(B11^2 - (C11*E4)^2)/($N$4*C11)</f>
+        <v>0.65660091653543506</v>
       </c>
       <c r="J11" s="6">
         <f>SQRT((C11*D4*$N$4)^2-(E11*(F4+F11))^2)/(E11*$N$4)</f>
-        <v>3.1271277336354317</v>
-      </c>
-      <c r="O11" s="21" t="s">
+        <v>3.1061464862190711</v>
+      </c>
+      <c r="O11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="23"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="20"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>28</v>
+      <c r="B12" s="12">
+        <v>93.4</v>
+      </c>
+      <c r="C12" s="4">
+        <f>C5</f>
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>33.22</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6">
+        <f>D5</f>
+        <v>0.74325358423915122</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="6" t="s">
-        <v>28</v>
+      <c r="I12" s="6">
+        <f>SQRT(B12^2 - (C12*E5)^2)/($N$4*C12)</f>
+        <v>0.73963910109570696</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M12" s="17"/>
+      <c r="M12" s="13"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="4">
-        <v>93</v>
+      <c r="B13" s="12">
+        <v>93.4</v>
       </c>
       <c r="C13" s="4">
         <v>0.8</v>
@@ -1061,27 +1095,62 @@
         <f>7</f>
         <v>7</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="12">
         <v>0.08</v>
       </c>
       <c r="F13" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="G13" s="6">
         <f>D6</f>
-        <v>0.37083101740411611</v>
+        <v>0.37162679211957561</v>
       </c>
       <c r="H13" s="6">
         <f>G13/SQRT(J13*I13)</f>
-        <v>0.32270857678250453</v>
+        <v>0.31940045686069785</v>
       </c>
       <c r="I13" s="6">
         <f>SQRT(B13^2 - (C13*E6)^2)/($N$4*C13)</f>
-        <v>0.362720540109012</v>
+        <v>0.36434404346222898</v>
       </c>
       <c r="J13" s="6">
         <f>SQRT((C13*D6*$N$4)^2-(E13*(F6+F13))^2)/(E13*$N$4)</f>
-        <v>3.6404824339996891</v>
+        <v>3.715620012081053</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="12">
+        <v>93.4</v>
+      </c>
+      <c r="C14" s="14">
+        <v>0.8</v>
+      </c>
+      <c r="D14" s="14">
+        <f>8.3</f>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <f>D7</f>
+        <v>0.37162679211957561</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="6">
+        <f>SQRT(B14^2 - (C14*E7)^2)/($N$4*C14)</f>
+        <v>0.36434404346222898</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PUTO EL QUE LEE
</commit_message>
<xml_diff>
--- a/TP4/Mediciones.xlsx
+++ b/TP4/Mediciones.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A98E50-955E-4297-BA73-BF492CEF3BAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F61DB52-3251-46F5-8A38-443E18DFC2D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parte 1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Caso</t>
   </si>
@@ -76,9 +76,6 @@
     <t>rad/s</t>
   </si>
   <si>
-    <t>V1 (V)</t>
-  </si>
-  <si>
     <t>I1 (A)</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>Se usaron cuentas en modulo</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Son electroimanes</t>
   </si>
   <si>
@@ -128,13 +122,16 @@
   </si>
   <si>
     <t>Sin núcleo (I2 = 0)</t>
+  </si>
+  <si>
+    <t>Hierro Sólido vacio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +141,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -205,7 +209,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -340,11 +344,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,6 +399,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -421,6 +442,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -703,13 +742,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -718,38 +757,33 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
-      <c r="M1" s="21" t="s">
+      <c r="M1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G2" s="5"/>
       <c r="M2" s="7" t="s">
         <v>8</v>
       </c>
@@ -761,27 +795,21 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14">
-        <v>93.4</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="D3" s="6">
-        <f>B3/($N$4*C3)</f>
-        <v>2.9730143369566049</v>
-      </c>
-      <c r="E3" s="14">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="32">
         <f>23</f>
         <v>23</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="32">
         <f>21.8</f>
         <v>21.8</v>
       </c>
+      <c r="G3" s="32"/>
       <c r="M3" s="7" t="s">
         <v>11</v>
       </c>
@@ -796,24 +824,12 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14">
-        <v>93.4</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.42</v>
-      </c>
-      <c r="D4" s="6">
-        <f>B4/($N$4*C4)</f>
-        <v>0.70786055641823931</v>
-      </c>
-      <c r="E4" s="14">
-        <f>23</f>
-        <v>23</v>
-      </c>
-      <c r="F4" s="14">
-        <f t="shared" ref="F4:F7" si="0">21.8</f>
-        <v>21.8</v>
-      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="16"/>
       <c r="M4" s="7" t="s">
         <v>14</v>
       </c>
@@ -826,99 +842,62 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="14">
-        <v>93.4</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="6">
-        <f>B5/($N$4*C5)</f>
-        <v>0.74325358423915122</v>
-      </c>
-      <c r="E5" s="14">
-        <f>23</f>
-        <v>23</v>
-      </c>
-      <c r="F5" s="14">
-        <f t="shared" si="0"/>
-        <v>21.8</v>
-      </c>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="14">
-        <v>93.4</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="D6" s="6">
-        <f>B6/($N$4*C6)</f>
-        <v>0.37162679211957561</v>
-      </c>
-      <c r="E6" s="14">
-        <f>23</f>
-        <v>23</v>
-      </c>
-      <c r="F6" s="14">
-        <f t="shared" si="0"/>
-        <v>21.8</v>
-      </c>
+      <c r="A6" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="14">
-        <v>93.4</v>
-      </c>
-      <c r="C7" s="14">
-        <v>0.8</v>
-      </c>
-      <c r="D7" s="6">
-        <f>B7/($N$4*C7)</f>
-        <v>0.37162679211957561</v>
-      </c>
-      <c r="E7" s="14">
-        <f>23</f>
-        <v>23</v>
-      </c>
-      <c r="F7" s="14">
-        <f t="shared" si="0"/>
-        <v>21.8</v>
-      </c>
-      <c r="G7" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="9"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="25" t="s">
+      <c r="A8" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="O8" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="O8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -928,13 +907,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>7</v>
@@ -946,17 +925,18 @@
         <v>3</v>
       </c>
       <c r="I9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="O9" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
+      <c r="K9" s="30"/>
+      <c r="O9" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -978,27 +958,27 @@
         <v>200</v>
       </c>
       <c r="G10" s="6">
-        <f>D3</f>
-        <v>2.9730143369566049</v>
+        <f>D10/(C10*$N$4)</f>
+        <v>0.15491081127611145</v>
       </c>
       <c r="H10" s="6">
         <f>G10/(SQRT(J10*I10))</f>
-        <v>0.77609519362771617</v>
+        <v>0.27608371263943349</v>
       </c>
       <c r="I10" s="6">
-        <f>SQRT(B10^2 - (C10*E3)^2)/($N$4*C10)</f>
+        <f>SQRT(B10^2 - (C10*E$3)^2)/($N$4*C10)</f>
         <v>0.98829680833112554</v>
       </c>
       <c r="J10" s="6">
-        <f>SQRT((C10*D3*$N$4)^2-(E10*(F3+F10))^2)/(E10*$N$4)</f>
-        <v>14.848296339954329</v>
-      </c>
-      <c r="O10" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="16"/>
-      <c r="R10" s="17"/>
+        <f>SQRT((C10*G10*$N$4)^2-(E10*(F$3+F10))^2)/(E10*$N$4)</f>
+        <v>0.31856238261710607</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="19"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -1023,27 +1003,26 @@
         <v>200</v>
       </c>
       <c r="G11" s="6">
-        <f>D4</f>
-        <v>0.70786055641823931</v>
+        <v>0.26</v>
       </c>
       <c r="H11" s="6">
         <f>G11/(SQRT(J11*I11))</f>
-        <v>0.49566243286548706</v>
+        <v>0.33219026191529116</v>
       </c>
       <c r="I11" s="6">
-        <f>SQRT(B11^2 - (C11*E4)^2)/($N$4*C11)</f>
+        <f t="shared" ref="I11:I14" si="0">SQRT(B11^2 - (C11*E$3)^2)/($N$4*C11)</f>
         <v>0.65660091653543506</v>
       </c>
       <c r="J11" s="6">
-        <f>SQRT((C11*D4*$N$4)^2-(E11*(F4+F11))^2)/(E11*$N$4)</f>
-        <v>3.1061464862190711</v>
-      </c>
-      <c r="O11" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="P11" s="19"/>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="20"/>
+        <f t="shared" ref="J11:J13" si="1">SQRT((C11*G11*$N$4)^2-(E11*(F$3+F11))^2)/(E11*$N$4)</f>
+        <v>0.93297803048255723</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="22"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -1053,7 +1032,6 @@
         <v>93.4</v>
       </c>
       <c r="C12" s="4">
-        <f>C5</f>
         <v>0.4</v>
       </c>
       <c r="D12" s="4">
@@ -1065,25 +1043,15 @@
       <c r="F12" s="3">
         <v>0</v>
       </c>
-      <c r="G12" s="6">
-        <f>D5</f>
-        <v>0.74325358423915122</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="6">
-        <f>SQRT(B12^2 - (C12*E5)^2)/($N$4*C12)</f>
-        <v>0.73963910109570696</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
       <c r="M12" s="13"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="12">
         <v>93.4</v>
@@ -1099,28 +1067,27 @@
         <v>0.08</v>
       </c>
       <c r="F13" s="3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G13" s="6">
-        <f>D6</f>
-        <v>0.37162679211957561</v>
+        <v>0.03</v>
       </c>
       <c r="H13" s="6">
         <f>G13/SQRT(J13*I13)</f>
-        <v>0.31940045686069785</v>
+        <v>6.2169899099559944E-2</v>
       </c>
       <c r="I13" s="6">
-        <f>SQRT(B13^2 - (C13*E6)^2)/($N$4*C13)</f>
+        <f t="shared" si="0"/>
         <v>0.36434404346222898</v>
       </c>
       <c r="J13" s="6">
-        <f>SQRT((C13*D6*$N$4)^2-(E13*(F6+F13))^2)/(E13*$N$4)</f>
-        <v>3.715620012081053</v>
+        <f>SQRT(ABS((C13*G13*$N$4)^2-(E13*(F$3+F13))^2))/(E13*$N$4)</f>
+        <v>0.63910249149638587</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" s="12">
         <v>93.4</v>
@@ -1138,20 +1105,34 @@
       <c r="F14" s="11">
         <v>0</v>
       </c>
-      <c r="G14" s="6">
-        <f>D7</f>
-        <v>0.37162679211957561</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14" s="6">
-        <f>SQRT(B14^2 - (C14*E7)^2)/($N$4*C14)</f>
-        <v>0.36434404346222898</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>28</v>
-      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="12">
+        <v>93.4</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0.35</v>
+      </c>
+      <c r="D15" s="16">
+        <v>16.5</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0</v>
+      </c>
+      <c r="F15" s="15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>